<commit_message>
affichage des notes bi2anwa3ih session normal et ratt GINF31 to GINF46
</commit_message>
<xml_diff>
--- a/Excel_files/Notes.xlsx
+++ b/Excel_files/Notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\PycharmProjects\PythonProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Application-Gestion-Note\App-Gestion-Notes\Excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044C084F-9A84-4E0D-9B51-6FE1109D1350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81286C51-6925-4CD5-BA3E-7D194810B3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
   <si>
     <t>CNE</t>
   </si>
@@ -39,9 +39,6 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>Lastname</t>
-  </si>
-  <si>
     <t>GINF31</t>
   </si>
   <si>
@@ -441,7 +438,7 @@
     <t>ZAHAR</t>
   </si>
   <si>
-    <t>Note</t>
+    <t>LastName</t>
   </si>
 </sst>
 </file>
@@ -476,7 +473,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -499,13 +496,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -813,7 +829,7 @@
   <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,57 +842,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="P1" s="3"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>21010395</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2">
         <v>13.32</v>
@@ -913,10 +927,6 @@
       </c>
       <c r="O2">
         <v>14.84</v>
-      </c>
-      <c r="P2">
-        <f>ROUND(AVERAGE(D2:O2),3)</f>
-        <v>13.423999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -924,10 +934,10 @@
         <v>21010278</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="D3">
         <v>12.57</v>
@@ -964,10 +974,6 @@
       </c>
       <c r="O3">
         <v>16.96</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P65" si="0">ROUND(AVERAGE(D3:O3),3)</f>
-        <v>12.455</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -975,10 +981,10 @@
         <v>21011326</v>
       </c>
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
       </c>
       <c r="D4">
         <v>13.32</v>
@@ -1015,10 +1021,6 @@
       </c>
       <c r="O4">
         <v>14.84</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -1026,10 +1028,10 @@
         <v>21010358</v>
       </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
       </c>
       <c r="D5">
         <v>13.32</v>
@@ -1066,10 +1068,6 @@
       </c>
       <c r="O5">
         <v>14.84</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>13.345000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1077,10 +1075,10 @@
         <v>21010266</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
       </c>
       <c r="D6">
         <v>15.33</v>
@@ -1117,10 +1115,6 @@
       </c>
       <c r="O6">
         <v>14.21</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>13.324</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -1128,10 +1122,10 @@
         <v>20001758</v>
       </c>
       <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
       </c>
       <c r="D7">
         <v>13.32</v>
@@ -1168,10 +1162,6 @@
       </c>
       <c r="O7">
         <v>14.84</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>13.493</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1179,10 +1169,10 @@
         <v>21010287</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
       </c>
       <c r="D8">
         <v>13.32</v>
@@ -1219,10 +1209,6 @@
       </c>
       <c r="O8">
         <v>14.84</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>12.795</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1230,10 +1216,10 @@
         <v>21010482</v>
       </c>
       <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
       <c r="D9">
         <v>13.32</v>
@@ -1270,10 +1256,6 @@
       </c>
       <c r="O9">
         <v>14.84</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>13.018000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1281,10 +1263,10 @@
         <v>21009157</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
       </c>
       <c r="D10">
         <v>13.32</v>
@@ -1321,10 +1303,6 @@
       </c>
       <c r="O10">
         <v>14.84</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>13.569000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1332,10 +1310,10 @@
         <v>21010356</v>
       </c>
       <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
       </c>
       <c r="D11">
         <v>13.32</v>
@@ -1372,10 +1350,6 @@
       </c>
       <c r="O11">
         <v>14.84</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>12.817</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1383,10 +1357,10 @@
         <v>21010411</v>
       </c>
       <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
       </c>
       <c r="D12">
         <v>13.32</v>
@@ -1423,10 +1397,6 @@
       </c>
       <c r="O12">
         <v>14.84</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1434,10 +1404,10 @@
         <v>21010476</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
       <c r="D13">
         <v>13.32</v>
@@ -1474,10 +1444,6 @@
       </c>
       <c r="O13">
         <v>14.84</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>13.478</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1485,10 +1451,10 @@
         <v>22012817</v>
       </c>
       <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
       <c r="D14">
         <v>13.32</v>
@@ -1525,10 +1491,6 @@
       </c>
       <c r="O14">
         <v>14.84</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>12.91</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -1536,10 +1498,10 @@
         <v>21009110</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
       </c>
       <c r="D15">
         <v>13.32</v>
@@ -1576,10 +1538,6 @@
       </c>
       <c r="O15">
         <v>14.84</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>13.173999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -1587,10 +1545,10 @@
         <v>21011779</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
       </c>
       <c r="D16">
         <v>13.32</v>
@@ -1628,20 +1586,16 @@
       <c r="O16">
         <v>14.84</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>14.242000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20011005</v>
       </c>
       <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
       </c>
       <c r="D17">
         <v>13.32</v>
@@ -1679,20 +1633,16 @@
       <c r="O17">
         <v>14.84</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>13.387</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21002603</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
       </c>
       <c r="D18">
         <v>13.32</v>
@@ -1730,20 +1680,16 @@
       <c r="O18">
         <v>14.84</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>12.942</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>21010261</v>
       </c>
       <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
       </c>
       <c r="D19">
         <v>13.32</v>
@@ -1781,20 +1727,16 @@
       <c r="O19">
         <v>14.84</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>13.478</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>21011724</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20">
         <v>13.32</v>
@@ -1832,20 +1774,16 @@
       <c r="O20">
         <v>14.84</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>13.532</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>21009025</v>
       </c>
       <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
         <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
       </c>
       <c r="D21">
         <v>13.32</v>
@@ -1883,20 +1821,16 @@
       <c r="O21">
         <v>14.84</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>12.853999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21010326</v>
       </c>
       <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
         <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
       </c>
       <c r="D22">
         <v>13.32</v>
@@ -1934,20 +1868,16 @@
       <c r="O22">
         <v>14.84</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>13.397</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21010299</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
       </c>
       <c r="D23">
         <v>13.32</v>
@@ -1985,20 +1915,16 @@
       <c r="O23">
         <v>14.84</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>12.885999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>21009475</v>
       </c>
       <c r="B24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" t="s">
         <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>59</v>
       </c>
       <c r="D24">
         <v>13.32</v>
@@ -2036,20 +1962,16 @@
       <c r="O24">
         <v>14.5</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>13.420999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21010439</v>
       </c>
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
         <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>61</v>
       </c>
       <c r="D25">
         <v>13.32</v>
@@ -2087,20 +2009,16 @@
       <c r="O25">
         <v>14.84</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>13.351000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21010403</v>
       </c>
       <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
         <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
       </c>
       <c r="D26">
         <v>13.32</v>
@@ -2138,20 +2056,16 @@
       <c r="O26">
         <v>14.84</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>13.218999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21010379</v>
       </c>
       <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
         <v>64</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
       </c>
       <c r="D27">
         <v>13.32</v>
@@ -2189,20 +2103,16 @@
       <c r="O27">
         <v>14.84</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>21010272</v>
       </c>
       <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s">
         <v>66</v>
-      </c>
-      <c r="C28" t="s">
-        <v>67</v>
       </c>
       <c r="D28">
         <v>13.32</v>
@@ -2240,20 +2150,16 @@
       <c r="O28">
         <v>14.84</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>13.455</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>21010324</v>
       </c>
       <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>68</v>
-      </c>
-      <c r="C29" t="s">
-        <v>69</v>
       </c>
       <c r="D29">
         <v>13.32</v>
@@ -2291,20 +2197,16 @@
       <c r="O29">
         <v>14.84</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20007042</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
       </c>
       <c r="D30">
         <v>13.32</v>
@@ -2342,20 +2244,16 @@
       <c r="O30">
         <v>14.84</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>21010274</v>
       </c>
       <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
         <v>72</v>
-      </c>
-      <c r="C31" t="s">
-        <v>73</v>
       </c>
       <c r="D31">
         <v>13.32</v>
@@ -2393,20 +2291,16 @@
       <c r="O31">
         <v>14.84</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>12.827</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>21010319</v>
       </c>
       <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
         <v>74</v>
-      </c>
-      <c r="C32" t="s">
-        <v>75</v>
       </c>
       <c r="D32">
         <v>13.32</v>
@@ -2444,20 +2338,16 @@
       <c r="O32">
         <v>14.84</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>13.827</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>19006658</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33">
         <v>6.42</v>
@@ -2495,20 +2385,16 @@
       <c r="O33">
         <v>14.37</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>13.105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>21010322</v>
       </c>
       <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" t="s">
         <v>77</v>
-      </c>
-      <c r="C34" t="s">
-        <v>78</v>
       </c>
       <c r="D34">
         <v>13.32</v>
@@ -2546,20 +2432,16 @@
       <c r="O34">
         <v>14.84</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>12.782999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>22012491</v>
       </c>
       <c r="B35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" t="s">
         <v>79</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
       </c>
       <c r="D35">
         <v>13.32</v>
@@ -2597,20 +2479,16 @@
       <c r="O35">
         <v>14.84</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>13.303000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>21010441</v>
       </c>
       <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" t="s">
         <v>81</v>
-      </c>
-      <c r="C36" t="s">
-        <v>82</v>
       </c>
       <c r="D36">
         <v>15.34</v>
@@ -2648,20 +2526,16 @@
       <c r="O36">
         <v>12.87</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>12.368</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>21010423</v>
       </c>
       <c r="B37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
         <v>83</v>
-      </c>
-      <c r="C37" t="s">
-        <v>84</v>
       </c>
       <c r="D37">
         <v>16.95</v>
@@ -2699,20 +2573,16 @@
       <c r="O37">
         <v>7.51</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="0"/>
-        <v>12.663</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20007896</v>
       </c>
       <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
         <v>85</v>
-      </c>
-      <c r="C38" t="s">
-        <v>86</v>
       </c>
       <c r="D38">
         <v>13.5</v>
@@ -2750,20 +2620,16 @@
       <c r="O38">
         <v>13.23</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>12.813000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>21011787</v>
       </c>
       <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
         <v>87</v>
-      </c>
-      <c r="C39" t="s">
-        <v>88</v>
       </c>
       <c r="D39">
         <v>10.94</v>
@@ -2801,20 +2667,16 @@
       <c r="O39">
         <v>8.31</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>12.487</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>21010306</v>
       </c>
       <c r="B40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
         <v>89</v>
-      </c>
-      <c r="C40" t="s">
-        <v>90</v>
       </c>
       <c r="D40">
         <v>13.32</v>
@@ -2852,20 +2714,16 @@
       <c r="O40">
         <v>14.84</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>21010320</v>
       </c>
       <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
         <v>91</v>
-      </c>
-      <c r="C41" t="s">
-        <v>92</v>
       </c>
       <c r="D41">
         <v>13.32</v>
@@ -2903,20 +2761,16 @@
       <c r="O41">
         <v>14.84</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="0"/>
-        <v>13.532999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>21010359</v>
       </c>
       <c r="B42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" t="s">
         <v>93</v>
-      </c>
-      <c r="C42" t="s">
-        <v>94</v>
       </c>
       <c r="D42">
         <v>13.32</v>
@@ -2954,20 +2808,16 @@
       <c r="O42">
         <v>14.84</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>12.952999999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>21010334</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D43">
         <v>13.32</v>
@@ -3005,20 +2855,16 @@
       <c r="O43">
         <v>14.84</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>13.718999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>21010011</v>
       </c>
       <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
         <v>96</v>
-      </c>
-      <c r="C44" t="s">
-        <v>97</v>
       </c>
       <c r="D44">
         <v>13.32</v>
@@ -3056,20 +2902,16 @@
       <c r="O44">
         <v>14.84</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="0"/>
-        <v>13.555</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>21010368</v>
       </c>
       <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
         <v>98</v>
-      </c>
-      <c r="C45" t="s">
-        <v>99</v>
       </c>
       <c r="D45">
         <v>13.32</v>
@@ -3107,20 +2949,16 @@
       <c r="O45">
         <v>14.84</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="0"/>
-        <v>13.135999999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>20009973</v>
       </c>
       <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" t="s">
         <v>100</v>
-      </c>
-      <c r="C46" t="s">
-        <v>101</v>
       </c>
       <c r="D46">
         <v>13.32</v>
@@ -3158,20 +2996,16 @@
       <c r="O46">
         <v>16.84</v>
       </c>
-      <c r="P46">
-        <f t="shared" si="0"/>
-        <v>12.837</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>21010231</v>
       </c>
       <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
         <v>102</v>
-      </c>
-      <c r="C47" t="s">
-        <v>103</v>
       </c>
       <c r="D47">
         <v>13.32</v>
@@ -3209,20 +3043,16 @@
       <c r="O47">
         <v>14.84</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>13.493</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>21011780</v>
       </c>
       <c r="B48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" t="s">
         <v>104</v>
-      </c>
-      <c r="C48" t="s">
-        <v>105</v>
       </c>
       <c r="D48">
         <v>13.39</v>
@@ -3260,20 +3090,16 @@
       <c r="O48">
         <v>8.9</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="0"/>
-        <v>12.134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>20000927</v>
       </c>
       <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
         <v>106</v>
-      </c>
-      <c r="C49" t="s">
-        <v>107</v>
       </c>
       <c r="D49">
         <v>13.32</v>
@@ -3311,20 +3137,16 @@
       <c r="O49">
         <v>14.84</v>
       </c>
-      <c r="P49">
-        <f t="shared" si="0"/>
-        <v>13.183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>20000104</v>
       </c>
       <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
         <v>108</v>
-      </c>
-      <c r="C50" t="s">
-        <v>109</v>
       </c>
       <c r="D50">
         <v>13.32</v>
@@ -3362,20 +3184,16 @@
       <c r="O50">
         <v>14.84</v>
       </c>
-      <c r="P50">
-        <f t="shared" si="0"/>
-        <v>13.375</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>21010740</v>
       </c>
       <c r="B51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" t="s">
         <v>110</v>
-      </c>
-      <c r="C51" t="s">
-        <v>111</v>
       </c>
       <c r="D51">
         <v>13.32</v>
@@ -3413,20 +3231,16 @@
       <c r="O51">
         <v>14.84</v>
       </c>
-      <c r="P51">
-        <f t="shared" si="0"/>
-        <v>13.933</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>21010291</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D52">
         <v>13.32</v>
@@ -3464,20 +3278,16 @@
       <c r="O52">
         <v>14.84</v>
       </c>
-      <c r="P52">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>21011784</v>
       </c>
       <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" t="s">
         <v>113</v>
-      </c>
-      <c r="C53" t="s">
-        <v>114</v>
       </c>
       <c r="D53">
         <v>11.89</v>
@@ -3515,20 +3325,16 @@
       <c r="O53">
         <v>9.7100000000000009</v>
       </c>
-      <c r="P53">
-        <f t="shared" si="0"/>
-        <v>12.019</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>21010332</v>
       </c>
       <c r="B54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" t="s">
         <v>115</v>
-      </c>
-      <c r="C54" t="s">
-        <v>116</v>
       </c>
       <c r="D54">
         <v>13.32</v>
@@ -3566,20 +3372,16 @@
       <c r="O54">
         <v>14.84</v>
       </c>
-      <c r="P54">
-        <f t="shared" si="0"/>
-        <v>13.635999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>20007695</v>
       </c>
       <c r="B55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" t="s">
         <v>117</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
       </c>
       <c r="D55">
         <v>13.32</v>
@@ -3617,20 +3419,16 @@
       <c r="O55">
         <v>14.84</v>
       </c>
-      <c r="P55">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>21010401</v>
       </c>
       <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" t="s">
         <v>119</v>
-      </c>
-      <c r="C56" t="s">
-        <v>120</v>
       </c>
       <c r="D56">
         <v>13.32</v>
@@ -3668,20 +3466,16 @@
       <c r="O56">
         <v>14.84</v>
       </c>
-      <c r="P56">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>21009322</v>
       </c>
       <c r="B57" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D57">
         <v>13.32</v>
@@ -3719,20 +3513,16 @@
       <c r="O57">
         <v>14.84</v>
       </c>
-      <c r="P57">
-        <f t="shared" si="0"/>
-        <v>13.467000000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>21011667</v>
       </c>
       <c r="B58" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" t="s">
         <v>122</v>
-      </c>
-      <c r="C58" t="s">
-        <v>123</v>
       </c>
       <c r="D58">
         <v>13.32</v>
@@ -3770,20 +3560,16 @@
       <c r="O58">
         <v>14.84</v>
       </c>
-      <c r="P58">
-        <f t="shared" si="0"/>
-        <v>13.243</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>21010348</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D59">
         <v>13.32</v>
@@ -3821,20 +3607,16 @@
       <c r="O59">
         <v>14.84</v>
       </c>
-      <c r="P59">
-        <f t="shared" si="0"/>
-        <v>13.292</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>21010242</v>
       </c>
       <c r="B60" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" t="s">
         <v>125</v>
-      </c>
-      <c r="C60" t="s">
-        <v>126</v>
       </c>
       <c r="D60">
         <v>13.32</v>
@@ -3872,20 +3654,16 @@
       <c r="O60">
         <v>14.84</v>
       </c>
-      <c r="P60">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>21015477</v>
       </c>
       <c r="B61" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" t="s">
         <v>127</v>
-      </c>
-      <c r="C61" t="s">
-        <v>128</v>
       </c>
       <c r="D61">
         <v>13.32</v>
@@ -3923,20 +3701,16 @@
       <c r="O61">
         <v>14.84</v>
       </c>
-      <c r="P61">
-        <f t="shared" si="0"/>
-        <v>13.827</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>20001713</v>
       </c>
       <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
         <v>129</v>
-      </c>
-      <c r="C62" t="s">
-        <v>130</v>
       </c>
       <c r="D62">
         <v>13.32</v>
@@ -3974,20 +3748,16 @@
       <c r="O62">
         <v>14.84</v>
       </c>
-      <c r="P62">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>21010255</v>
       </c>
       <c r="B63" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" t="s">
         <v>131</v>
-      </c>
-      <c r="C63" t="s">
-        <v>132</v>
       </c>
       <c r="D63">
         <v>7.31</v>
@@ -4025,20 +3795,16 @@
       <c r="O63">
         <v>15.82</v>
       </c>
-      <c r="P63">
-        <f t="shared" si="0"/>
-        <v>12.314</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>21011615</v>
       </c>
       <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
         <v>133</v>
-      </c>
-      <c r="C64" t="s">
-        <v>134</v>
       </c>
       <c r="D64">
         <v>13.32</v>
@@ -4076,20 +3842,16 @@
       <c r="O64">
         <v>14.84</v>
       </c>
-      <c r="P64">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>21010409</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D65">
         <v>13.32</v>
@@ -4126,10 +3888,6 @@
       </c>
       <c r="O65">
         <v>14.84</v>
-      </c>
-      <c r="P65">
-        <f t="shared" si="0"/>
-        <v>13.577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>